<commit_message>
add import excel template
</commit_message>
<xml_diff>
--- a/TaiLieu/HocVienImportTemplate.xlsx
+++ b/TaiLieu/HocVienImportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anhlq\source\repos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B813ECAE-48A3-4AFB-B23B-AE71A630E4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC120A0B-4087-45E2-B928-26D5A56D6CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5C998386-A175-4F64-A353-2CC329544C84}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{5C998386-A175-4F64-A353-2CC329544C84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Mã học viên</t>
   </si>
@@ -74,23 +74,35 @@
     <t>ID xã</t>
   </si>
   <si>
-    <t>test@gmail.com</t>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>1234567891</t>
+  </si>
+  <si>
+    <t>0123456790</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>0123456789</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
+    <t>1234567890</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +119,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -473,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556651CE-A9FB-428A-9761-E23409581807}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,46 +553,86 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1234567890</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1234567890</v>
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F2" s="2">
         <v>1234567890</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{62CE32CE-FDF3-4204-814B-CBC84B106854}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{A8716455-B81A-4234-ABCC-E5E4C9561135}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>